<commit_message>
Supervisor Feedback, Background research extracts added
</commit_message>
<xml_diff>
--- a/Gantt Chart/Sample_Gantt/Gantt_created_in_excel.xlsx
+++ b/Gantt Chart/Sample_Gantt/Gantt_created_in_excel.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="330" windowWidth="18720" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="330" windowWidth="18720" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Gantt Chart steps using date" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -47,7 +48,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -132,10 +133,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -223,8 +224,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="92711552"/>
-        <c:axId val="92907392"/>
+        <c:axId val="58498048"/>
+        <c:axId val="73257728"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="bar"/>
@@ -292,24 +293,24 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="116774784"/>
-        <c:axId val="113184128"/>
+        <c:axId val="73265152"/>
+        <c:axId val="73259264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92711552"/>
+        <c:axId val="58498048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92907392"/>
+        <c:crossAx val="73257728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92907392"/>
+        <c:axId val="73257728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -317,12 +318,12 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92711552"/>
+        <c:crossAx val="58498048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113184128"/>
+        <c:axId val="73259264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="37047"/>
@@ -331,19 +332,20 @@
         <c:axPos val="t"/>
         <c:numFmt formatCode="dd/mm/yy;@" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116774784"/>
+        <c:crossAx val="73265152"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="116774784"/>
+        <c:axId val="73265152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113184128"/>
+        <c:crossAx val="73259264"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -357,7 +359,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -599,11 +601,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="118309248"/>
-        <c:axId val="118310784"/>
+        <c:axId val="73328896"/>
+        <c:axId val="73797632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118309248"/>
+        <c:axId val="73328896"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -620,14 +622,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118310784"/>
+        <c:crossAx val="73797632"/>
         <c:crossesAt val="36533"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118310784"/>
+        <c:axId val="73797632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="37300"/>
@@ -647,7 +649,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118309248"/>
+        <c:crossAx val="73328896"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="60"/>
@@ -669,11 +671,183 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.85401732231394678"/>
-          <c:y val="0.51332360519155285"/>
-          <c:w val="0.10358434934127354"/>
+          <c:y val="0.51332360519155273"/>
+          <c:w val="0.10358434934127356"/>
           <c:h val="4.4239543451563966E-2"/>
         </c:manualLayout>
       </c:layout>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Task 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Task 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Task 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Task 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Task 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mm/yy;@</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>36533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36876</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37047</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Completed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="47133056"/>
+        <c:axId val="47134592"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="47133056"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="47134592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="47134592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="37047"/>
+          <c:min val="36533"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[$-809]dd\ mmmm\ yyyy;@" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-2700000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="47133056"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="60"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -689,16 +863,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>514350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -750,6 +924,1678 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419102</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>186753</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="20" name="Group 19"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1028702" y="104775"/>
+          <a:ext cx="5863651" cy="1076326"/>
+          <a:chOff x="1028702" y="104775"/>
+          <a:chExt cx="5863651" cy="1076326"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="TextBox 1"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1028702" y="276227"/>
+            <a:ext cx="2390774" cy="257174"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>1. Insert</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> a 2-D bar chart (Stacked bar).</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="1025" name="Picture 1"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="3928047" y="104775"/>
+            <a:ext cx="2964306" cy="1076326"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="1">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="21" name="Group 20"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1047751" y="1514475"/>
+          <a:ext cx="6553200" cy="1343026"/>
+          <a:chOff x="1047751" y="1514475"/>
+          <a:chExt cx="6553200" cy="1343026"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="TextBox 5"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1047751" y="1714502"/>
+            <a:ext cx="3533773" cy="495298"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>2.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> Right click on the bar chart and click "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Select Data</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>".</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>3. Click "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Add</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>" from the wizard (on the left).</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="1026" name="Picture 2"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="4752975" y="1514475"/>
+            <a:ext cx="2847976" cy="1343026"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="1">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>16083</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="22" name="Group 21"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1171576" y="3238501"/>
+          <a:ext cx="5638800" cy="1159082"/>
+          <a:chOff x="1085851" y="3076576"/>
+          <a:chExt cx="5638800" cy="1159082"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="TextBox 7"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1085851" y="3200402"/>
+            <a:ext cx="3533773" cy="819148"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>4. Select the field under</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Series </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" u="sng" baseline="0"/>
+              <a:t>n</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" u="none" baseline="0"/>
+              <a:t>ame".</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>5.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> Select the desired table header (on the same sheet or navigate to apporiate sheet). Or you can give it any name you like.</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="1027" name="Picture 3"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+          <a:srcRect r="33642" b="35586"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="4943475" y="3076576"/>
+            <a:ext cx="1781176" cy="1159082"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="1">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>117680</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="23" name="Group 22"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="942976" y="4972050"/>
+          <a:ext cx="5880304" cy="3810000"/>
+          <a:chOff x="942976" y="4972050"/>
+          <a:chExt cx="5880304" cy="3810000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="1028" name="Picture 4"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="5025820" y="4972050"/>
+            <a:ext cx="1797460" cy="3810000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="1">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="TextBox 10"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1038226" y="5210177"/>
+            <a:ext cx="3533773" cy="685798"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>6. Select the field under</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Series </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" u="sng" baseline="0"/>
+              <a:t>v</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" u="none" baseline="0"/>
+              <a:t>alues".</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>7.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> Select the desired data.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t>8. Press "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>OK</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>"</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="TextBox 11"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="942976" y="8458202"/>
+            <a:ext cx="3533773" cy="295273"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>9. Select</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> all desired data using steps 3-8.</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>122158</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>400051</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>77868</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="24" name="Group 23"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="914401" y="9266158"/>
+          <a:ext cx="7410450" cy="1670210"/>
+          <a:chOff x="952501" y="9189958"/>
+          <a:chExt cx="7410450" cy="1670210"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="1029" name="Picture 5"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="5114925" y="9189958"/>
+            <a:ext cx="3248026" cy="1670210"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="1">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="TextBox 13"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="952501" y="9296401"/>
+            <a:ext cx="3533773" cy="1247774"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>10. Now</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> to select the vertical Axis Label (I know it's confusing as it says Horizontal on the wizard!), select </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>"Edit" </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> on the right panel. Then select the range of data (as in step 7) that you want to be displayed as vertical labels. This will lay the data in order of Bottom-up on the chart, we will fix this later.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>154452</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>64624</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="Group 24"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="762001" y="11393952"/>
+          <a:ext cx="8105774" cy="3720172"/>
+          <a:chOff x="762001" y="11393952"/>
+          <a:chExt cx="8105774" cy="3720172"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="TextBox 14"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="762001" y="11734801"/>
+            <a:ext cx="3533773" cy="1019174"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>11. You can now see the data</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> on the chart</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>. If for some reason, one of the data category doesn't show up, it may be overshadowed by the other data category. In this case, use the "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>arrow</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>" on the left panel to move the order of the data.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="1030" name="Picture 6"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="4829175" y="11393952"/>
+            <a:ext cx="4038600" cy="3720172"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="1">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="31" name="Group 30"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="752476" y="15535275"/>
+          <a:ext cx="10496549" cy="4257675"/>
+          <a:chOff x="752476" y="15535275"/>
+          <a:chExt cx="10496549" cy="4257675"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="1031" name="Picture 7"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="5019675" y="15535275"/>
+            <a:ext cx="2657475" cy="4238625"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="1">
+            <a:noFill/>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd type="none" w="med" len="med"/>
+          </a:ln>
+          <a:effectLst/>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="TextBox 17"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="752476" y="15887701"/>
+            <a:ext cx="3533773" cy="1019174"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>12. To correct the display order of the vertical Axis</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> labels, select the vertical Axis group and right click to select </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>"Format Axis"</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>.</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>13. Select  "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" u="sng" baseline="0"/>
+              <a:t>C</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" u="none" baseline="0"/>
+              <a:t>ategories in reverse order</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" u="none" baseline="0"/>
+              <a:t>"</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> and "At maximum cate</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" u="sng" baseline="0"/>
+              <a:t>g</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" u="none" baseline="0"/>
+              <a:t>ory</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>" as depicted.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="19" name="Picture 18"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+          <a:srcRect l="1795" t="5587" r="13846" b="11173"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8115300" y="15535275"/>
+            <a:ext cx="3133725" cy="4257675"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>42025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>81801</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="35" name="Group 34"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="447676" y="20616025"/>
+          <a:ext cx="10201274" cy="1373276"/>
+          <a:chOff x="447676" y="20616025"/>
+          <a:chExt cx="10201274" cy="1373276"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="30" name="TextBox 29"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="447676" y="20650201"/>
+            <a:ext cx="3533773" cy="1019174"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>14. To display</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> the horizontal Axis in desired Date range, first take the corresponding numeric value of the highest and the lowest date. This is done by right clicking on the cell, selecting "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Format Cells"</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> , then selecting "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>General"</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="32" name="Picture 31"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5114925" y="20706838"/>
+            <a:ext cx="2771776" cy="1124974"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="33" name="Picture 32"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8210550" y="20616025"/>
+            <a:ext cx="2438400" cy="1373276"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="42" name="Group 41"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="581025" y="22774275"/>
+          <a:ext cx="11353799" cy="2800350"/>
+          <a:chOff x="581025" y="22774275"/>
+          <a:chExt cx="11353799" cy="2800350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="34" name="TextBox 33"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="581025" y="23012401"/>
+            <a:ext cx="3533773" cy="1438274"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>15. Select</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> the horizontal Axis group, right click to select "</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Format Axis" </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> (as in step 12).</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>16. Enter the numeric values noted in step 14 for the dates in the </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Axis Options</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> -&gt; </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Minimum</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Maximum</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> fields. Enter a </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Major Unit</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>, this is the interval in days between displayed dates (60 days in this example).</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>17. Choose the desired date format from </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> -&gt; </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Date</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t>  as depicted.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="36" name="Picture 35"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+          <a:srcRect r="6459" b="55307"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4886324" y="22869525"/>
+            <a:ext cx="3724275" cy="2286000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="37" name="Picture 36"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+          <a:srcRect r="26555" b="45251"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9010649" y="22774275"/>
+            <a:ext cx="2924175" cy="2800350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="43" name="Group 42"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="371476" y="26355675"/>
+          <a:ext cx="7191374" cy="3086100"/>
+          <a:chOff x="371476" y="26355675"/>
+          <a:chExt cx="7191374" cy="3086100"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="38" name="Picture 37"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+          <a:srcRect r="24654" b="39665"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4448175" y="26355675"/>
+            <a:ext cx="3114675" cy="3086100"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="41" name="TextBox 40"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="371476" y="26946226"/>
+            <a:ext cx="3533773" cy="761999"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>18. To</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> display the dates on the horizontal axis diagonally, select </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Alignment</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> from and enter -45 in the </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Custom angle</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> field as depicted.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="47" name="Group 46"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="419100" y="30622875"/>
+          <a:ext cx="14344650" cy="3752850"/>
+          <a:chOff x="419100" y="30622875"/>
+          <a:chExt cx="14344650" cy="3752850"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="39" name="Picture 38"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4171950" y="30622875"/>
+            <a:ext cx="4752975" cy="2895600"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="40" name="Picture 39"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9401175" y="30680025"/>
+            <a:ext cx="5362575" cy="3695700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="45" name="TextBox 44"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="419100" y="31413450"/>
+            <a:ext cx="3533773" cy="761999"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>19. Finally to make</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+              <a:t> it look like a Gantt Chart, hide the unrelated data by selecting the data block in the bar chart and setting its </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>Fill</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> to </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+              <a:t>No Fill</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100" i="0" baseline="0"/>
+              <a:t> as depicted.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1100" i="1" baseline="0"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1042,7 +2888,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1152,7 +3000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
@@ -1161,4 +3009,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="E174" sqref="E174"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>